<commit_message>
Updated solution template with catalog number
</commit_message>
<xml_diff>
--- a/Solution_recipes/Solution_Recipe_Template.xlsx
+++ b/Solution_recipes/Solution_Recipe_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregMilburn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregMilburn\Documents\github\Protocols\Solution_recipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D30094A-F41E-4C8D-B5E0-DFB86B790594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CE6F1F-C662-4740-81F2-CBFD3EAA91B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="-16440" windowWidth="29040" windowHeight="15720" xr2:uid="{FF8B8365-E929-431C-A409-6ED40BA60103}"/>
+    <workbookView xWindow="-14040" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FF8B8365-E929-431C-A409-6ED40BA60103}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Solution Name</t>
   </si>
@@ -263,18 +263,27 @@
   <si>
     <t>Notes:</t>
   </si>
+  <si>
+    <t>Catalog #</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -488,82 +497,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,413 +894,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF85ED49-DFE3-4719-87F3-E23436E6CD7A}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="4" width="14.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="G1" s="22" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="H1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="19"/>
-    </row>
-    <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="25"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
       <c r="M2" s="19"/>
-    </row>
-    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28"/>
-    </row>
-    <row r="5" spans="1:16" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="22"/>
+    </row>
+    <row r="5" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="J5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="K5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="L5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="M5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="N5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="O5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="P5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="Q5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F6" s="1" t="e">
-        <f>D6/E6</f>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="e">
+        <f>E6/F6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H6" s="1" t="e">
-        <f>G6*F6*1</f>
+      <c r="I6" s="1" t="e">
+        <f>H6*G6*1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="1" t="e">
-        <f>G6*F6*0.5</f>
+      <c r="K6" s="1" t="e">
+        <f>H6*G6*0.5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="1" t="e">
-        <f>G6*F6*0.25</f>
+      <c r="M6" s="1" t="e">
+        <f>H6*G6*0.25</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="1" t="e">
-        <f>G6*F6*0.1</f>
+      <c r="O6" s="1" t="e">
+        <f>H6*G6*0.1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="H10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="I10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="J10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="K10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="L10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="M10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="N10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="O10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="P10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="Q10" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H11" s="1" t="e">
-        <f>((1*G11)/F11)*1000</f>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="e">
+        <f>((1*H11)/G11)*1000</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="1" t="e">
-        <f>((0.5*G11)/F11)*1000</f>
+      <c r="K11" s="1" t="e">
+        <f>((0.5*H11)/G11)*1000</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="1" t="e">
-        <f>((0.25*G11)/F11)*1000</f>
+      <c r="M11" s="1" t="e">
+        <f>((0.25*H11)/G11)*1000</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N11" s="1" t="e">
-        <f>((0.1*G11)/F11)*1000</f>
+      <c r="O11" s="1" t="e">
+        <f>((0.1*H11)/G11)*1000</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="29"/>
+      <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="F14" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="29"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="2"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="C16" s="29"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A19:P25"/>
-    <mergeCell ref="G1:L3"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A19:Q25"/>
+    <mergeCell ref="H1:M3"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
some thoughts on the notes
</commit_message>
<xml_diff>
--- a/Solution_recipes/Solution_Recipe_Template.xlsx
+++ b/Solution_recipes/Solution_Recipe_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GregMilburn\Documents\github\Protocols\Solution_recipes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\utku\GitHub\Protocols\Solution_recipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CE6F1F-C662-4740-81F2-CBFD3EAA91B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25352A1-6A6C-4255-99C5-9BD9C0051A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14040" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FF8B8365-E929-431C-A409-6ED40BA60103}"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="13800" xr2:uid="{FF8B8365-E929-431C-A409-6ED40BA60103}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Solution Name</t>
   </si>
@@ -265,6 +265,54 @@
   </si>
   <si>
     <t>Catalog #</t>
+  </si>
+  <si>
+    <t>Compound:</t>
+  </si>
+  <si>
+    <t>Company:</t>
+  </si>
+  <si>
+    <t>Catalog #:</t>
+  </si>
+  <si>
+    <t>Lot #:</t>
+  </si>
+  <si>
+    <t>MW:</t>
+  </si>
+  <si>
+    <t>% purity:</t>
+  </si>
+  <si>
+    <t>Corrected MW:</t>
+  </si>
+  <si>
+    <t>Final Conc (M):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the chemical substance </t>
+  </si>
+  <si>
+    <t>Name of the manufacturer</t>
+  </si>
+  <si>
+    <t>Serial number of the product</t>
+  </si>
+  <si>
+    <t>The identification number assigned to a batch of chemicals by the manufacturer</t>
+  </si>
+  <si>
+    <t>Molecular weight of the chemical substance</t>
+  </si>
+  <si>
+    <t>Final concentration in Moles</t>
+  </si>
+  <si>
+    <t>Molecular weight correction for the impurities</t>
+  </si>
+  <si>
+    <t>Measurement of the quality of the chemical substance. This information is found in the certificate of analysis for each lot</t>
   </si>
 </sst>
 </file>
@@ -497,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -525,9 +573,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -573,7 +618,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,88 +957,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF85ED49-DFE3-4719-87F3-E23436E6CD7A}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B27" sqref="B27:H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="19.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="H1" s="14" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="H1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="16"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="15"/>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="19"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="18"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="22"/>
-    </row>
-    <row r="5" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="21"/>
+    </row>
+    <row r="5" spans="1:17" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1028,7 +1091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G6" s="1" t="e">
         <f>E6/F6</f>
         <v>#DIV/0!</v>
@@ -1062,7 +1125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -1115,7 +1178,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I11" s="1" t="e">
         <f>((1*H11)/G11)*1000</f>
         <v>#DIV/0!</v>
@@ -1145,181 +1208,239 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="29"/>
       <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="24"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="29"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F15" s="24"/>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="29"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+    </row>
+    <row r="25" spans="1:17" ht="30.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="30"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="30"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A19:Q25"/>
+  <mergeCells count="14">
+    <mergeCell ref="B27:H27"/>
     <mergeCell ref="H1:M3"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>